<commit_message>
Added # Cases per 1M (Cumulative)
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\covid-19-au-vaccinations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7563164-AA94-4A15-938E-599D7353EFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D669436-EFBA-43D2-BBBC-50A6CA77CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="111">
   <si>
     <t># Cases (7-day avg)</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>NNDSS</t>
+  </si>
+  <si>
+    <t># Cases per 1M (Cumulative)</t>
   </si>
 </sst>
 </file>
@@ -924,8 +927,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:G96" totalsRowShown="0">
-  <autoFilter ref="A1:G96" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:G97" totalsRowShown="0">
+  <autoFilter ref="A1:G97" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Metric Catergory"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Metric Catergory - Sort"/>
@@ -1236,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E5" sqref="E5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1351,7 +1354,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -1359,7 +1362,12 @@
       <c r="E5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -1369,7 +1377,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -1387,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>60</v>
@@ -1395,12 +1403,7 @@
       <c r="E7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
@@ -1410,7 +1413,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>70</v>
@@ -1419,6 +1422,9 @@
         <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1430,7 +1436,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>80</v>
@@ -1438,7 +1444,9 @@
       <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -1448,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>90</v>
@@ -1456,9 +1464,7 @@
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -1468,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -1476,7 +1482,9 @@
       <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -1486,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -1494,9 +1502,7 @@
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -1506,7 +1512,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13">
         <v>120</v>
@@ -1526,16 +1532,15 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>130</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1547,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15">
         <v>140</v>
@@ -1568,7 +1573,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -1581,27 +1586,28 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D17">
         <v>160</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>170</v>
@@ -1621,7 +1627,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>180</v>
@@ -1641,7 +1647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20">
         <v>190</v>
@@ -1661,7 +1667,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <v>200</v>
@@ -1681,7 +1687,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>210</v>
@@ -1701,7 +1707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>220</v>
@@ -1721,7 +1727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24">
         <v>230</v>
@@ -1741,7 +1747,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1749,17 +1755,19 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D25">
         <v>240</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1767,7 +1775,7 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26">
         <v>250</v>
@@ -1777,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1785,7 +1793,7 @@
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27">
         <v>260</v>
@@ -1795,27 +1803,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <v>270</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29">
         <v>280</v>
@@ -1835,7 +1841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30">
         <v>290</v>
@@ -1855,7 +1861,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31">
         <v>300</v>
@@ -1875,7 +1881,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1883,7 +1889,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D32">
         <v>310</v>
@@ -1903,7 +1909,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33">
         <v>320</v>
@@ -1923,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34">
         <v>330</v>
@@ -1943,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35">
         <v>340</v>
@@ -1963,7 +1969,7 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36">
         <v>350</v>
@@ -1983,7 +1989,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37">
         <v>360</v>
@@ -2003,7 +2009,7 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38">
         <v>370</v>
@@ -2022,13 +2028,15 @@
       <c r="B39">
         <v>30</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>97</v>
+      <c r="C39" t="s">
+        <v>29</v>
       </c>
       <c r="D39">
         <v>380</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>42</v>
       </c>
@@ -2041,7 +2049,7 @@
         <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40">
         <v>390</v>
@@ -2059,7 +2067,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41">
         <v>400</v>
@@ -2077,7 +2085,7 @@
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42">
         <v>410</v>
@@ -2095,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <v>420</v>
@@ -2113,7 +2121,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44">
         <v>430</v>
@@ -2131,7 +2139,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45">
         <v>440</v>
@@ -2149,7 +2157,7 @@
         <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D46">
         <v>450</v>
@@ -2167,7 +2175,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47">
         <v>460</v>
@@ -2185,7 +2193,7 @@
         <v>30</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48">
         <v>470</v>
@@ -2203,7 +2211,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49">
         <v>480</v>
@@ -2221,7 +2229,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50">
         <v>490</v>
@@ -2233,20 +2241,18 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
         <v>30</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D51">
         <v>500</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
         <v>42</v>
       </c>
@@ -2259,7 +2265,7 @@
         <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52">
         <v>510</v>
@@ -2279,7 +2285,7 @@
         <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53">
         <v>520</v>
@@ -2299,7 +2305,7 @@
         <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54">
         <v>530</v>
@@ -2307,7 +2313,9 @@
       <c r="E54" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
@@ -2317,7 +2325,7 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55">
         <v>540</v>
@@ -2335,7 +2343,7 @@
         <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D56">
         <v>550</v>
@@ -2353,7 +2361,7 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D57">
         <v>560</v>
@@ -2361,9 +2369,7 @@
       <c r="E57" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
@@ -2373,7 +2379,7 @@
         <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58">
         <v>570</v>
@@ -2387,13 +2393,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B59">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D59">
         <v>580</v>
@@ -2401,7 +2407,9 @@
       <c r="E59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F59" s="1"/>
+      <c r="F59" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
@@ -2411,7 +2419,7 @@
         <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D60">
         <v>590</v>
@@ -2429,7 +2437,7 @@
         <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D61">
         <v>600</v>
@@ -2447,7 +2455,7 @@
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D62">
         <v>610</v>
@@ -2459,21 +2467,21 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63">
-        <v>60</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
       </c>
       <c r="D63">
         <v>620</v>
       </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
@@ -2483,7 +2491,7 @@
         <v>60</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D64">
         <v>630</v>
@@ -2501,7 +2509,7 @@
         <v>60</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D65">
         <v>640</v>
@@ -2519,7 +2527,7 @@
         <v>60</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D66">
         <v>650</v>
@@ -2537,7 +2545,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D67">
         <v>660</v>
@@ -2555,7 +2563,7 @@
         <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D68">
         <v>670</v>
@@ -2573,7 +2581,7 @@
         <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D69">
         <v>680</v>
@@ -2591,7 +2599,7 @@
         <v>60</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D70">
         <v>690</v>
@@ -2609,7 +2617,7 @@
         <v>60</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D71">
         <v>700</v>
@@ -2627,7 +2635,7 @@
         <v>60</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D72">
         <v>710</v>
@@ -2645,7 +2653,7 @@
         <v>60</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D73">
         <v>720</v>
@@ -2663,7 +2671,7 @@
         <v>60</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D74">
         <v>730</v>
@@ -2681,7 +2689,7 @@
         <v>60</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D75">
         <v>740</v>
@@ -2699,7 +2707,7 @@
         <v>60</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76">
         <v>750</v>
@@ -2716,8 +2724,8 @@
       <c r="B77">
         <v>60</v>
       </c>
-      <c r="C77" t="s">
-        <v>58</v>
+      <c r="C77" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D77">
         <v>760</v>
@@ -2735,7 +2743,7 @@
         <v>60</v>
       </c>
       <c r="C78" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D78">
         <v>770</v>
@@ -2753,7 +2761,7 @@
         <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79">
         <v>780</v>
@@ -2771,7 +2779,7 @@
         <v>60</v>
       </c>
       <c r="C80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D80">
         <v>790</v>
@@ -2788,8 +2796,8 @@
       <c r="B81">
         <v>60</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>84</v>
+      <c r="C81" t="s">
+        <v>62</v>
       </c>
       <c r="D81">
         <v>800</v>
@@ -2807,7 +2815,7 @@
         <v>60</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D82">
         <v>810</v>
@@ -2825,7 +2833,7 @@
         <v>60</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D83">
         <v>820</v>
@@ -2843,7 +2851,7 @@
         <v>60</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D84">
         <v>830</v>
@@ -2861,7 +2869,7 @@
         <v>60</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D85">
         <v>840</v>
@@ -2879,7 +2887,7 @@
         <v>60</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D86">
         <v>850</v>
@@ -2897,7 +2905,7 @@
         <v>60</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D87">
         <v>860</v>
@@ -2909,13 +2917,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B88">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D88">
         <v>870</v>
@@ -2933,7 +2941,7 @@
         <v>70</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D89">
         <v>880</v>
@@ -2951,7 +2959,7 @@
         <v>70</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D90">
         <v>890</v>
@@ -2969,7 +2977,7 @@
         <v>70</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D91">
         <v>900</v>
@@ -2987,7 +2995,7 @@
         <v>70</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D92">
         <v>910</v>
@@ -3005,7 +3013,7 @@
         <v>70</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D93">
         <v>920</v>
@@ -3022,8 +3030,8 @@
       <c r="B94">
         <v>70</v>
       </c>
-      <c r="C94" t="s">
-        <v>72</v>
+      <c r="C94" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D94">
         <v>930</v>
@@ -3041,7 +3049,7 @@
         <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D95">
         <v>940</v>
@@ -3059,13 +3067,31 @@
         <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D96">
         <v>950</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>59</v>
+      </c>
+      <c r="B97">
+        <v>70</v>
+      </c>
+      <c r="C97" t="s">
+        <v>74</v>
+      </c>
+      <c r="D97">
+        <v>960</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added # Cases (1-year rolling average)
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\covid-19-au-vaccinations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D669436-EFBA-43D2-BBBC-50A6CA77CC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB1A1B-E0F6-4F35-AEAB-D1BAB6762F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="112">
   <si>
     <t># Cases (7-day avg)</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t># Cases per 1M (Cumulative)</t>
+  </si>
+  <si>
+    <t># Cases (1-year rolling average)</t>
   </si>
 </sst>
 </file>
@@ -927,8 +930,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:G97" totalsRowShown="0">
-  <autoFilter ref="A1:G97" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:G98" totalsRowShown="0">
+  <autoFilter ref="A1:G98" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Metric Catergory"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Metric Catergory - Sort"/>
@@ -1239,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:G5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1413,7 +1416,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="D8">
         <v>70</v>
@@ -1436,7 +1439,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>80</v>
@@ -1445,6 +1448,9 @@
         <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1456,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>90</v>
@@ -1464,7 +1470,9 @@
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
@@ -1474,7 +1482,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>100</v>
@@ -1482,9 +1490,7 @@
       <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -1494,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>110</v>
@@ -1502,7 +1508,9 @@
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
@@ -1512,7 +1520,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>120</v>
@@ -1520,9 +1528,7 @@
       <c r="E13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
@@ -1532,7 +1538,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>130</v>
@@ -1552,16 +1558,15 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>140</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1573,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16">
         <v>150</v>
@@ -1594,7 +1599,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17">
         <v>160</v>
@@ -1609,21 +1614,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <v>170</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1635,7 +1641,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>180</v>
@@ -1655,7 +1661,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>190</v>
@@ -1675,7 +1681,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>200</v>
@@ -1695,7 +1701,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>210</v>
@@ -1715,7 +1721,7 @@
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>220</v>
@@ -1735,7 +1741,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24">
         <v>230</v>
@@ -1755,7 +1761,7 @@
         <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25">
         <v>240</v>
@@ -1775,14 +1781,16 @@
         <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D26">
         <v>250</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <v>0</v>
+      <c r="E26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
@@ -1793,7 +1801,7 @@
         <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27">
         <v>260</v>
@@ -1811,7 +1819,7 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28">
         <v>270</v>
@@ -1823,22 +1831,20 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D29">
         <v>280</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>42</v>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -1849,7 +1855,7 @@
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30">
         <v>290</v>
@@ -1869,7 +1875,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31">
         <v>300</v>
@@ -1889,7 +1895,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32">
         <v>310</v>
@@ -1909,7 +1915,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>320</v>
@@ -1929,7 +1935,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34">
         <v>330</v>
@@ -1949,7 +1955,7 @@
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35">
         <v>340</v>
@@ -1969,7 +1975,7 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36">
         <v>350</v>
@@ -1989,7 +1995,7 @@
         <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37">
         <v>360</v>
@@ -2009,7 +2015,7 @@
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38">
         <v>370</v>
@@ -2029,7 +2035,7 @@
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39">
         <v>380</v>
@@ -2048,13 +2054,15 @@
       <c r="B40">
         <v>30</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>97</v>
+      <c r="C40" t="s">
+        <v>29</v>
       </c>
       <c r="D40">
         <v>390</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>42</v>
       </c>
@@ -2067,7 +2075,7 @@
         <v>30</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41">
         <v>400</v>
@@ -2085,7 +2093,7 @@
         <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D42">
         <v>410</v>
@@ -2103,7 +2111,7 @@
         <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43">
         <v>420</v>
@@ -2121,7 +2129,7 @@
         <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44">
         <v>430</v>
@@ -2139,7 +2147,7 @@
         <v>30</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D45">
         <v>440</v>
@@ -2157,7 +2165,7 @@
         <v>30</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D46">
         <v>450</v>
@@ -2175,7 +2183,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47">
         <v>460</v>
@@ -2193,7 +2201,7 @@
         <v>30</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D48">
         <v>470</v>
@@ -2211,7 +2219,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D49">
         <v>480</v>
@@ -2229,7 +2237,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50">
         <v>490</v>
@@ -2247,7 +2255,7 @@
         <v>30</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D51">
         <v>500</v>
@@ -2259,20 +2267,18 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>40</v>
-      </c>
-      <c r="C52" t="s">
         <v>30</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D52">
         <v>510</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
         <v>42</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D53">
         <v>520</v>
@@ -2305,7 +2311,7 @@
         <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54">
         <v>530</v>
@@ -2325,7 +2331,7 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55">
         <v>540</v>
@@ -2333,7 +2339,9 @@
       <c r="E55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
@@ -2343,7 +2351,7 @@
         <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56">
         <v>550</v>
@@ -2361,7 +2369,7 @@
         <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D57">
         <v>560</v>
@@ -2379,7 +2387,7 @@
         <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D58">
         <v>570</v>
@@ -2387,9 +2395,7 @@
       <c r="E58" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
@@ -2399,7 +2405,7 @@
         <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D59">
         <v>580</v>
@@ -2413,13 +2419,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B60">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="D60">
         <v>590</v>
@@ -2427,7 +2433,9 @@
       <c r="E60" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
@@ -2437,7 +2445,7 @@
         <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D61">
         <v>600</v>
@@ -2455,7 +2463,7 @@
         <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D62">
         <v>610</v>
@@ -2473,7 +2481,7 @@
         <v>50</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D63">
         <v>620</v>
@@ -2485,21 +2493,21 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64">
-        <v>60</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="C64" t="s">
+        <v>39</v>
       </c>
       <c r="D64">
         <v>630</v>
       </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
@@ -2509,7 +2517,7 @@
         <v>60</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D65">
         <v>640</v>
@@ -2527,7 +2535,7 @@
         <v>60</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66">
         <v>650</v>
@@ -2545,7 +2553,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D67">
         <v>660</v>
@@ -2563,7 +2571,7 @@
         <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D68">
         <v>670</v>
@@ -2581,7 +2589,7 @@
         <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D69">
         <v>680</v>
@@ -2599,7 +2607,7 @@
         <v>60</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D70">
         <v>690</v>
@@ -2617,7 +2625,7 @@
         <v>60</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D71">
         <v>700</v>
@@ -2635,7 +2643,7 @@
         <v>60</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D72">
         <v>710</v>
@@ -2653,7 +2661,7 @@
         <v>60</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D73">
         <v>720</v>
@@ -2671,7 +2679,7 @@
         <v>60</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D74">
         <v>730</v>
@@ -2689,7 +2697,7 @@
         <v>60</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D75">
         <v>740</v>
@@ -2707,7 +2715,7 @@
         <v>60</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D76">
         <v>750</v>
@@ -2725,7 +2733,7 @@
         <v>60</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D77">
         <v>760</v>
@@ -2742,8 +2750,8 @@
       <c r="B78">
         <v>60</v>
       </c>
-      <c r="C78" t="s">
-        <v>58</v>
+      <c r="C78" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D78">
         <v>770</v>
@@ -2761,7 +2769,7 @@
         <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D79">
         <v>780</v>
@@ -2779,7 +2787,7 @@
         <v>60</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80">
         <v>790</v>
@@ -2797,7 +2805,7 @@
         <v>60</v>
       </c>
       <c r="C81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D81">
         <v>800</v>
@@ -2814,8 +2822,8 @@
       <c r="B82">
         <v>60</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>84</v>
+      <c r="C82" t="s">
+        <v>62</v>
       </c>
       <c r="D82">
         <v>810</v>
@@ -2833,7 +2841,7 @@
         <v>60</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D83">
         <v>820</v>
@@ -2851,7 +2859,7 @@
         <v>60</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D84">
         <v>830</v>
@@ -2869,7 +2877,7 @@
         <v>60</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D85">
         <v>840</v>
@@ -2887,7 +2895,7 @@
         <v>60</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D86">
         <v>850</v>
@@ -2905,7 +2913,7 @@
         <v>60</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D87">
         <v>860</v>
@@ -2923,7 +2931,7 @@
         <v>60</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D88">
         <v>870</v>
@@ -2935,13 +2943,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B89">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D89">
         <v>880</v>
@@ -2959,7 +2967,7 @@
         <v>70</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D90">
         <v>890</v>
@@ -2977,7 +2985,7 @@
         <v>70</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D91">
         <v>900</v>
@@ -2995,7 +3003,7 @@
         <v>70</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D92">
         <v>910</v>
@@ -3013,7 +3021,7 @@
         <v>70</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D93">
         <v>920</v>
@@ -3031,7 +3039,7 @@
         <v>70</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D94">
         <v>930</v>
@@ -3048,8 +3056,8 @@
       <c r="B95">
         <v>70</v>
       </c>
-      <c r="C95" t="s">
-        <v>72</v>
+      <c r="C95" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D95">
         <v>940</v>
@@ -3067,7 +3075,7 @@
         <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D96">
         <v>950</v>
@@ -3085,13 +3093,31 @@
         <v>70</v>
       </c>
       <c r="C97" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D97">
         <v>960</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98">
+        <v>70</v>
+      </c>
+      <c r="C98" t="s">
+        <v>74</v>
+      </c>
+      <c r="D98">
+        <v>970</v>
+      </c>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Data Source: ABS
</commit_message>
<xml_diff>
--- a/Metrics.xlsx
+++ b/Metrics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\covid-19-au-vaccinations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB1A1B-E0F6-4F35-AEAB-D1BAB6762F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6093615-CAF2-4855-9A67-2A35B031C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="119">
   <si>
     <t># Cases (7-day avg)</t>
   </si>
@@ -369,6 +369,27 @@
   </si>
   <si>
     <t># Cases (1-year rolling average)</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t># Registered deaths - COVID-19</t>
+  </si>
+  <si>
+    <t># Registered deaths - Influenza</t>
+  </si>
+  <si>
+    <t># Registered deaths - RSV</t>
+  </si>
+  <si>
+    <t># Registered deaths - COVID-19 (Cumulative)</t>
+  </si>
+  <si>
+    <t># Registered deaths - Influenza (Cumulative)</t>
+  </si>
+  <si>
+    <t># Registered deaths - RSV (Cumulative)</t>
   </si>
 </sst>
 </file>
@@ -930,9 +951,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:G98" totalsRowShown="0">
-  <autoFilter ref="A1:G98" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Metrics" displayName="Metrics" ref="A1:H104" totalsRowShown="0">
+  <autoFilter ref="A1:H104" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Metric Catergory"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Metric Catergory - Sort"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Metric"/>
@@ -940,6 +961,7 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="covidlive.com.au" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="health.gov.au" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{A095DB30-0F8C-474D-82E2-320F2AB838E7}" name="NNDSS"/>
+    <tableColumn id="8" xr3:uid="{D93DE384-1004-486B-9129-9F3D64E78D44}" name="ABS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1242,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1257,7 +1279,7 @@
     <col min="5" max="5" width="14.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1279,8 +1301,11 @@
       <c r="G1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1303,7 +1328,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1326,7 +1351,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1349,7 +1374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1372,7 +1397,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1390,7 +1415,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1408,7 +1433,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1431,7 +1456,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1454,7 +1479,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1474,7 +1499,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1492,7 +1517,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1512,7 +1537,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1530,7 +1555,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1550,7 +1575,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1570,7 +1595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2211,7 +2236,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2229,7 +2254,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2247,7 +2272,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2265,7 +2290,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2283,121 +2308,121 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s">
         <v>30</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="D53">
         <v>520</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54">
-        <v>40</v>
-      </c>
-      <c r="C54" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D54">
         <v>530</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55">
-        <v>40</v>
-      </c>
-      <c r="C55" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="D55">
         <v>540</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56">
-        <v>40</v>
-      </c>
-      <c r="C56" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="D56">
         <v>550</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H56" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57">
-        <v>40</v>
-      </c>
-      <c r="C57" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D57">
         <v>560</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H57" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58">
-        <v>40</v>
-      </c>
-      <c r="C58" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D58">
         <v>570</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H58" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -2405,7 +2430,7 @@
         <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="D59">
         <v>580</v>
@@ -2417,7 +2442,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2425,7 +2450,7 @@
         <v>40</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="D60">
         <v>590</v>
@@ -2437,15 +2462,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B61">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D61">
         <v>600</v>
@@ -2453,17 +2478,19 @@
       <c r="E61" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F61" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B62">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D62">
         <v>610</v>
@@ -2473,15 +2500,15 @@
       </c>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B63">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D63">
         <v>620</v>
@@ -2491,15 +2518,15 @@
       </c>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B64">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D64">
         <v>630</v>
@@ -2511,111 +2538,115 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B65">
-        <v>60</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="C65" t="s">
+        <v>70</v>
       </c>
       <c r="D65">
         <v>640</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B66">
-        <v>60</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
       </c>
       <c r="D66">
         <v>650</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B67">
-        <v>60</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
+      </c>
+      <c r="C67" t="s">
+        <v>35</v>
       </c>
       <c r="D67">
         <v>660</v>
       </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B68">
-        <v>60</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
+      </c>
+      <c r="C68" t="s">
+        <v>37</v>
       </c>
       <c r="D68">
         <v>670</v>
       </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B69">
-        <v>60</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>75</v>
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
       </c>
       <c r="D69">
         <v>680</v>
       </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E69" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70">
-        <v>60</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>39</v>
       </c>
       <c r="D70">
         <v>690</v>
       </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E70" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
@@ -2625,7 +2656,7 @@
         <v>60</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D71">
         <v>700</v>
@@ -2643,7 +2674,7 @@
         <v>60</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D72">
         <v>710</v>
@@ -2661,7 +2692,7 @@
         <v>60</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D73">
         <v>720</v>
@@ -2679,7 +2710,7 @@
         <v>60</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D74">
         <v>730</v>
@@ -2697,7 +2728,7 @@
         <v>60</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D75">
         <v>740</v>
@@ -2715,7 +2746,7 @@
         <v>60</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D76">
         <v>750</v>
@@ -2733,7 +2764,7 @@
         <v>60</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D77">
         <v>760</v>
@@ -2751,7 +2782,7 @@
         <v>60</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D78">
         <v>770</v>
@@ -2768,8 +2799,8 @@
       <c r="B79">
         <v>60</v>
       </c>
-      <c r="C79" t="s">
-        <v>58</v>
+      <c r="C79" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D79">
         <v>780</v>
@@ -2786,8 +2817,8 @@
       <c r="B80">
         <v>60</v>
       </c>
-      <c r="C80" t="s">
-        <v>60</v>
+      <c r="C80" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D80">
         <v>790</v>
@@ -2804,8 +2835,8 @@
       <c r="B81">
         <v>60</v>
       </c>
-      <c r="C81" t="s">
-        <v>61</v>
+      <c r="C81" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D81">
         <v>800</v>
@@ -2822,8 +2853,8 @@
       <c r="B82">
         <v>60</v>
       </c>
-      <c r="C82" t="s">
-        <v>62</v>
+      <c r="C82" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D82">
         <v>810</v>
@@ -2841,7 +2872,7 @@
         <v>60</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D83">
         <v>820</v>
@@ -2859,7 +2890,7 @@
         <v>60</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D84">
         <v>830</v>
@@ -2876,8 +2907,8 @@
       <c r="B85">
         <v>60</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>86</v>
+      <c r="C85" t="s">
+        <v>58</v>
       </c>
       <c r="D85">
         <v>840</v>
@@ -2894,8 +2925,8 @@
       <c r="B86">
         <v>60</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>87</v>
+      <c r="C86" t="s">
+        <v>60</v>
       </c>
       <c r="D86">
         <v>850</v>
@@ -2912,8 +2943,8 @@
       <c r="B87">
         <v>60</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>88</v>
+      <c r="C87" t="s">
+        <v>61</v>
       </c>
       <c r="D87">
         <v>860</v>
@@ -2930,8 +2961,8 @@
       <c r="B88">
         <v>60</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>89</v>
+      <c r="C88" t="s">
+        <v>62</v>
       </c>
       <c r="D88">
         <v>870</v>
@@ -2949,7 +2980,7 @@
         <v>60</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D89">
         <v>880</v>
@@ -2961,13 +2992,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B90">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D90">
         <v>890</v>
@@ -2979,13 +3010,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B91">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D91">
         <v>900</v>
@@ -2997,13 +3028,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B92">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D92">
         <v>910</v>
@@ -3015,13 +3046,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B93">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D93">
         <v>920</v>
@@ -3033,13 +3064,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B94">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D94">
         <v>930</v>
@@ -3051,13 +3082,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B95">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D95">
         <v>940</v>
@@ -3074,8 +3105,8 @@
       <c r="B96">
         <v>70</v>
       </c>
-      <c r="C96" t="s">
-        <v>72</v>
+      <c r="C96" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="D96">
         <v>950</v>
@@ -3092,8 +3123,8 @@
       <c r="B97">
         <v>70</v>
       </c>
-      <c r="C97" t="s">
-        <v>73</v>
+      <c r="C97" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="D97">
         <v>960</v>
@@ -3110,14 +3141,122 @@
       <c r="B98">
         <v>70</v>
       </c>
-      <c r="C98" t="s">
-        <v>74</v>
+      <c r="C98" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D98">
         <v>970</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>59</v>
+      </c>
+      <c r="B99">
+        <v>70</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D99">
+        <v>980</v>
+      </c>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>59</v>
+      </c>
+      <c r="B100">
+        <v>70</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100">
+        <v>990</v>
+      </c>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>59</v>
+      </c>
+      <c r="B101">
+        <v>70</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D101">
+        <v>1000</v>
+      </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>59</v>
+      </c>
+      <c r="B102">
+        <v>70</v>
+      </c>
+      <c r="C102" t="s">
+        <v>72</v>
+      </c>
+      <c r="D102">
+        <v>1010</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>59</v>
+      </c>
+      <c r="B103">
+        <v>70</v>
+      </c>
+      <c r="C103" t="s">
+        <v>73</v>
+      </c>
+      <c r="D103">
+        <v>1020</v>
+      </c>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>59</v>
+      </c>
+      <c r="B104">
+        <v>70</v>
+      </c>
+      <c r="C104" t="s">
+        <v>74</v>
+      </c>
+      <c r="D104">
+        <v>1030</v>
+      </c>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>